<commit_message>
color coded session protocol demo
</commit_message>
<xml_diff>
--- a/user-interface-design/Background_Animation_Summary.xlsx
+++ b/user-interface-design/Background_Animation_Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/work/trans-ionospheric/user-interface-design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{EED8FCCF-BA2C-D94C-959B-9BE038C61126}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{5413FDDB-78E4-5446-B8E0-12822507FA4C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14000" yWindow="5100" windowWidth="34500" windowHeight="20880" xr2:uid="{2CE80556-C01F-DF4C-80BA-89C303F71068}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="42">
   <si>
     <t>Time</t>
   </si>
@@ -87,18 +87,6 @@
     <t>channel list transmitted</t>
   </si>
   <si>
-    <t>REGISTER</t>
-  </si>
-  <si>
-    <t>401 unauthorized</t>
-  </si>
-  <si>
-    <t>REGISTER + login</t>
-  </si>
-  <si>
-    <t>200 OK</t>
-  </si>
-  <si>
     <t>radio off</t>
   </si>
   <si>
@@ -109,6 +97,60 @@
   </si>
   <si>
     <t>channel assigned</t>
+  </si>
+  <si>
+    <t>off</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Aqua</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>channel list decoded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Green </t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>REGISTER tx</t>
+  </si>
+  <si>
+    <t>REGISTER rx</t>
+  </si>
+  <si>
+    <t>401 unauthorized decide</t>
+  </si>
+  <si>
+    <t>401 unauthorized tx</t>
+  </si>
+  <si>
+    <t>REGISTER+login tx</t>
+  </si>
+  <si>
+    <t>REGISTER+login rx</t>
+  </si>
+  <si>
+    <t>200 OK decide</t>
+  </si>
+  <si>
+    <t>200 OK tx</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>RTP media traffic</t>
+  </si>
+  <si>
+    <t>flicker</t>
   </si>
 </sst>
 </file>
@@ -127,12 +169,48 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59996337778862885"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59996337778862885"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39994506668294322"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -147,15 +225,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFEC3536"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -464,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93E969CB-6BF7-A147-82D6-D7B93363D940}">
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="U41" sqref="U41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -531,10 +621,55 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -544,21 +679,156 @@
       <c r="B3" s="1">
         <v>3.4722222222222222E-5</v>
       </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1">
         <v>4.6296296296296294E-5</v>
       </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="O4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1">
         <v>8.1018518518518516E-5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="O5" t="s">
+        <v>24</v>
+      </c>
+      <c r="P5" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
@@ -568,6 +838,51 @@
       <c r="B6" s="1">
         <v>9.2592592592592588E-5</v>
       </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M6" t="s">
+        <v>24</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="O6" t="s">
+        <v>24</v>
+      </c>
+      <c r="P6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -576,43 +891,799 @@
       <c r="B7" s="1">
         <v>1.1574074074074073E-4</v>
       </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" t="s">
+        <v>24</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B8" s="1">
-        <v>1.7361111111111112E-4</v>
+        <v>1.273148148148148E-4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M8" t="s">
+        <v>24</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P8" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B9" s="1">
-        <v>1.8518518518518518E-4</v>
+        <v>1.6203703703703703E-4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M9" t="s">
+        <v>24</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B10" s="1">
-        <v>2.199074074074074E-4</v>
+        <v>1.7361111111111112E-4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M10" t="s">
+        <v>24</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1">
-        <v>2.3148148148148146E-4</v>
+        <v>1.8518518518518518E-4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M11" t="s">
+        <v>24</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1.9675925925925926E-4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="I12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M12" t="s">
+        <v>24</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q12" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2.199074074074074E-4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M13" t="s">
+        <v>24</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2.199074074074074E-4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M14" t="s">
+        <v>24</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.8518518518518518E-4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M15" t="s">
+        <v>24</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1.9675925925925926E-4</v>
+      </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M16" t="s">
+        <v>24</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2.6620370370370372E-4</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" t="s">
+        <v>24</v>
+      </c>
+      <c r="I17" t="s">
+        <v>24</v>
+      </c>
+      <c r="J17" t="s">
+        <v>24</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P17" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="1">
+        <v>3.2407407407407406E-4</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18" t="s">
+        <v>24</v>
+      </c>
+      <c r="H18" t="s">
+        <v>24</v>
+      </c>
+      <c r="I18" t="s">
+        <v>24</v>
+      </c>
+      <c r="J18" t="s">
+        <v>24</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P18" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="1">
+        <v>3.2407407407407406E-4</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" t="s">
+        <v>24</v>
+      </c>
+      <c r="J19" t="s">
+        <v>24</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P19" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="1">
+        <v>3.2407407407407406E-4</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" t="s">
+        <v>24</v>
+      </c>
+      <c r="H20" t="s">
+        <v>24</v>
+      </c>
+      <c r="I20" t="s">
+        <v>24</v>
+      </c>
+      <c r="J20" t="s">
+        <v>24</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P20" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="1">
+        <v>3.2407407407407406E-4</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H21" t="s">
+        <v>24</v>
+      </c>
+      <c r="I21" t="s">
+        <v>24</v>
+      </c>
+      <c r="J21" t="s">
+        <v>24</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P21" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>